<commit_message>
final commit after changes
</commit_message>
<xml_diff>
--- a/MyShopProject/src/test/resources/TestData/TestData1.xlsx
+++ b/MyShopProject/src/test/resources/TestData/TestData1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{44D22A43-9ED7-4C02-B995-0A121FA5C530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D98AE44-F3B6-4AAA-85BC-6B18E8B359CB}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{44D22A43-9ED7-4C02-B995-0A121FA5C530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F03409EE-FD67-4302-9D85-799369BAFFD5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="ProductDetails" sheetId="4" r:id="rId4"/>
     <sheet name="SearchProduct" sheetId="6" r:id="rId5"/>
     <sheet name="AccountCreationData" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="95">
   <si>
     <t>TestCases</t>
   </si>
@@ -189,12 +190,6 @@
     <t>qty</t>
   </si>
   <si>
-    <t>t-shirt</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>ghfsdtyfg@gmail.com</t>
   </si>
   <si>
@@ -282,19 +277,40 @@
     <t>ABCDEF</t>
   </si>
   <si>
-    <t>newtest1@gmail.com</t>
-  </si>
-  <si>
-    <t>newtest2@gmail.com</t>
-  </si>
-  <si>
-    <t>newtest3@gmail.com</t>
-  </si>
-  <si>
     <t>admin@2909.com</t>
   </si>
   <si>
     <t>aawsum2909</t>
+  </si>
+  <si>
+    <t>dresses</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>1986</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>jddjysj</t>
+  </si>
+  <si>
+    <t>hssuujg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr </t>
+  </si>
+  <si>
+    <t>newtest31@gmail.com</t>
+  </si>
+  <si>
+    <t>newtest32@gmail.com</t>
+  </si>
+  <si>
+    <t>newtest33@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1047,10 +1063,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1082,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1080,7 +1098,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1097,7 +1115,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1115,13 +1133,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B2" s="6">
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1152,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,7 +1164,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1156,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,201 +1190,110 @@
     <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="O1" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="C3" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" s="11" t="s">
+      <c r="H3" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="E4" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="H4" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1377,4 +1304,120 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BE6C27-BE3D-4DF1-AD4B-4FB3E2791F47}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>